<commit_message>
upd xlsx format add WhyCancel task celery add download file to report change Index.html
</commit_message>
<xml_diff>
--- a/print_service_app/xlsx/export_dispatcher.xlsx
+++ b/print_service_app/xlsx/export_dispatcher.xlsx
@@ -3001,12 +3001,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20240704-1</t>
+          <t>20240716-1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>04.07.2024</t>
+          <t>16.07.2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -3080,7 +3080,11 @@
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>16.07.2024</t>
+        </is>
+      </c>
       <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="inlineStr"/>
     </row>

</xml_diff>